<commit_message>
pseudo rebase desde la rama de alvaro
</commit_message>
<xml_diff>
--- a/generador_ruta_critica/MallaCurricular.xlsx
+++ b/generador_ruta_critica/MallaCurricular.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador ruta critica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador_ruta_critica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469C103-951B-4783-84BE-390636E3E435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285A9E4-41C0-45A2-8E1F-0B12872E6960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
   <si>
     <t>CBM1000</t>
   </si>
@@ -51,21 +51,6 @@
     <t>FIC1000</t>
   </si>
   <si>
-    <t>Algebra y Geometria</t>
-  </si>
-  <si>
-    <t>Calculo 1</t>
-  </si>
-  <si>
-    <t>Quimica</t>
-  </si>
-  <si>
-    <t>Programacion</t>
-  </si>
-  <si>
-    <t>Comu. Para la ingenieria</t>
-  </si>
-  <si>
     <t>CBM1002</t>
   </si>
   <si>
@@ -78,24 +63,6 @@
     <t>CIT1010</t>
   </si>
   <si>
-    <t>CFG1</t>
-  </si>
-  <si>
-    <t>Algebra lineal</t>
-  </si>
-  <si>
-    <t>Calculo 2</t>
-  </si>
-  <si>
-    <t>Mecanica</t>
-  </si>
-  <si>
-    <t>Programacion avanzada</t>
-  </si>
-  <si>
-    <t>CFG 1</t>
-  </si>
-  <si>
     <t>CBM1005</t>
   </si>
   <si>
@@ -111,21 +78,6 @@
     <t>CIT2100</t>
   </si>
   <si>
-    <t>Ec. Diferenciales</t>
-  </si>
-  <si>
-    <t>Calculo 3</t>
-  </si>
-  <si>
-    <t>Calor y Ondas</t>
-  </si>
-  <si>
-    <t>Estructura de Datos</t>
-  </si>
-  <si>
-    <t>Redes de datos</t>
-  </si>
-  <si>
     <t>CIT2204</t>
   </si>
   <si>
@@ -138,153 +90,66 @@
     <t>CIT2001</t>
   </si>
   <si>
-    <t>CFG2</t>
-  </si>
-  <si>
     <t>FIC1001</t>
   </si>
   <si>
-    <t>Prob. Y estadistica</t>
-  </si>
-  <si>
-    <t>Metodos numericos</t>
-  </si>
-  <si>
-    <t>Electricidad y Magnetismo</t>
-  </si>
-  <si>
-    <t>Diseño y Analisis de algoritmos</t>
-  </si>
-  <si>
-    <t>CFG 2</t>
-  </si>
-  <si>
-    <t>Ingles 1</t>
-  </si>
-  <si>
     <t>CII2750</t>
   </si>
   <si>
-    <t>Optimizacion</t>
-  </si>
-  <si>
     <t>CIT2106</t>
   </si>
   <si>
-    <t>Electronica y Electrotecnia</t>
-  </si>
-  <si>
     <t>CIT2200</t>
   </si>
   <si>
-    <t>Proyecto TICS 1</t>
-  </si>
-  <si>
     <t>CIT2002</t>
   </si>
   <si>
-    <t>Bases de Datos</t>
-  </si>
-  <si>
-    <t>CFG3</t>
-  </si>
-  <si>
-    <t>CFG 3</t>
-  </si>
-  <si>
     <t>FIC1002</t>
   </si>
   <si>
-    <t>Ingles 2</t>
-  </si>
-  <si>
     <t>CII2000</t>
   </si>
   <si>
-    <t>Introduccion a la Economia</t>
-  </si>
-  <si>
     <t>CIT2202</t>
   </si>
   <si>
-    <t>Modelos Estoc. Y simulación</t>
-  </si>
-  <si>
     <t>CIT2101</t>
   </si>
   <si>
-    <t>Señales y Sistemas</t>
-  </si>
-  <si>
     <t>CIT2003</t>
   </si>
   <si>
-    <t>Sistemas Operativos</t>
-  </si>
-  <si>
     <t>CIT2103</t>
   </si>
   <si>
-    <t>Sistemas Digitales</t>
-  </si>
-  <si>
     <t>CII1000</t>
   </si>
   <si>
-    <t>Contabilidad y Costos</t>
-  </si>
-  <si>
     <t>CIT2005</t>
   </si>
   <si>
-    <t>Ingenieria de Software</t>
-  </si>
-  <si>
     <t>CIT2102</t>
   </si>
   <si>
-    <t>Comunicaciones Digitales</t>
-  </si>
-  <si>
     <t>FIC1003</t>
   </si>
   <si>
-    <t>Derecho en Ingenieria</t>
-  </si>
-  <si>
     <t>CIT2104</t>
   </si>
   <si>
-    <t>Arquitectura de Computadores</t>
-  </si>
-  <si>
     <t>CIT2203</t>
   </si>
   <si>
-    <t>Gestión Organizacional</t>
-  </si>
-  <si>
     <t>CIT2004</t>
   </si>
   <si>
-    <t>Arquitectura de Sistemas</t>
-  </si>
-  <si>
     <t>CIT2105</t>
   </si>
   <si>
-    <t>Cripto. Y seguridad en Redes</t>
-  </si>
-  <si>
     <t>CIT2201</t>
   </si>
   <si>
-    <t>Proyecto TICS 2</t>
-  </si>
-  <si>
-    <t>CFG4</t>
-  </si>
-  <si>
     <t>Electivo Profesional</t>
   </si>
   <si>
@@ -300,9 +165,6 @@
     <t>CIT3200</t>
   </si>
   <si>
-    <t>Evaluación de Proyectos TIC</t>
-  </si>
-  <si>
     <t>CIT33XX-2</t>
   </si>
   <si>
@@ -318,9 +180,6 @@
     <t>CIT3201</t>
   </si>
   <si>
-    <t>Proyectos TICS 3</t>
-  </si>
-  <si>
     <t>CIT33XX-4</t>
   </si>
   <si>
@@ -330,52 +189,172 @@
     <t>Nombre Asignatura</t>
   </si>
   <si>
-    <t>Prerrequisito</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>CBM1002 - CBM1003</t>
-  </si>
-  <si>
-    <t>CBM1003 - CBF1000</t>
-  </si>
-  <si>
-    <t>CBM1005 -CBM1006</t>
-  </si>
-  <si>
-    <t>CBM1002 - CBM1006</t>
-  </si>
-  <si>
-    <t>CIT2100 - CIT 2001</t>
-  </si>
-  <si>
-    <t>CIT2100 - CIT2204 - CII2750</t>
-  </si>
-  <si>
-    <t>CIT2204 - CIT2106</t>
-  </si>
-  <si>
-    <t>CIT2100 - CIT2002</t>
-  </si>
-  <si>
-    <t>CIT2200 - CIT2002</t>
-  </si>
-  <si>
-    <t>CIT2200 - CIT2005 - CIT2102</t>
-  </si>
-  <si>
-    <t>CII1000 - CIT2201</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Semestre</t>
   </si>
   <si>
-    <t>NULL</t>
+    <t>Abre la/s asignatura/s:</t>
+  </si>
+  <si>
+    <t>11, 17, 22</t>
+  </si>
+  <si>
+    <t>7, 8, 33</t>
+  </si>
+  <si>
+    <t>11, 12, 13, 16, 17</t>
+  </si>
+  <si>
+    <t>14, 15</t>
+  </si>
+  <si>
+    <t>18, 22, 28</t>
+  </si>
+  <si>
+    <t>24, 29, 31</t>
+  </si>
+  <si>
+    <t>29, 30</t>
+  </si>
+  <si>
+    <t>24, 25</t>
+  </si>
+  <si>
+    <t>30, 32</t>
+  </si>
+  <si>
+    <t>34, 41</t>
+  </si>
+  <si>
+    <t>31, 35</t>
+  </si>
+  <si>
+    <t>39, 41</t>
+  </si>
+  <si>
+    <t>CFG</t>
+  </si>
+  <si>
+    <t>MECÁNICA</t>
+  </si>
+  <si>
+    <t>CALOR Y ONDAS</t>
+  </si>
+  <si>
+    <t>ELECTRICIDAD Y MAGNETISMO</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA Y GEOMETRÍA</t>
+  </si>
+  <si>
+    <t>CÁLCULO I</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA LINEAL</t>
+  </si>
+  <si>
+    <t>CÁLCULO II</t>
+  </si>
+  <si>
+    <t>ECUACIONES DIFERENCIALES</t>
+  </si>
+  <si>
+    <t>CÁLCULO III</t>
+  </si>
+  <si>
+    <t>MÉTODOS NUMÉRICOS</t>
+  </si>
+  <si>
+    <t>QUÍMICA</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD Y COSTOS</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN A LA ECONOMÍA</t>
+  </si>
+  <si>
+    <t>OPTIMIZACIÓN</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN AVANZADA</t>
+  </si>
+  <si>
+    <t>ESTRUCTURAS DE DATOS</t>
+  </si>
+  <si>
+    <t>DISEÑO Y ANÁLISIS DE ALGORITMOS</t>
+  </si>
+  <si>
+    <t>BASES DE DATOS</t>
+  </si>
+  <si>
+    <t>SISTEMAS OPERATIVOS</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA DE SISTEMAS</t>
+  </si>
+  <si>
+    <t>INGENIERÍA DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>REDES DE DATOS</t>
+  </si>
+  <si>
+    <t>SEÑALES Y SISTEMAS</t>
+  </si>
+  <si>
+    <t>COMUNICACIONES DIGITALES</t>
+  </si>
+  <si>
+    <t>SISTEMAS DIGITALES</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA DE COMPUTADORES</t>
+  </si>
+  <si>
+    <t>CRIPTOGRAFÍA Y SEGURIDAD EN REDES</t>
+  </si>
+  <si>
+    <t>PROYECTO EN TICS I</t>
+  </si>
+  <si>
+    <t>PROYECTO EN TICS II</t>
+  </si>
+  <si>
+    <t>MODELOS ESTOCASTICOS Y SIMULACIÓN</t>
+  </si>
+  <si>
+    <t>GESTIÓN ORGANIZACIÓNAL</t>
+  </si>
+  <si>
+    <t>EVALUACIÓN DE PROYECTOS TIC</t>
+  </si>
+  <si>
+    <t>PROYECTO EN TICS III</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN PARA LA INGENIERÍA</t>
+  </si>
+  <si>
+    <t>INGLÉS I</t>
+  </si>
+  <si>
+    <t>INGLÉS II</t>
+  </si>
+  <si>
+    <t>DERECHO EN INGENIERÍA</t>
+  </si>
+  <si>
+    <t>PROBABILIDADES Y ESTADÍSTICAS</t>
+  </si>
+  <si>
+    <t>ELECTRÓNICA Y ELECTROTECNIA</t>
   </si>
 </sst>
 </file>
@@ -523,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -536,16 +515,36 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -875,7 +874,7 @@
   <dimension ref="A2:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,23 +884,24 @@
     <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -912,12 +912,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="12">
+        <v>70</v>
+      </c>
+      <c r="D3" s="12">
+        <v>6</v>
+      </c>
+      <c r="E3" s="32">
         <v>1</v>
       </c>
     </row>
@@ -929,12 +929,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="12">
+        <v>71</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="32">
         <v>1</v>
       </c>
     </row>
@@ -946,12 +946,12 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="12">
+        <v>77</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
         <v>1</v>
       </c>
     </row>
@@ -963,12 +963,12 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="12">
+        <v>81</v>
+      </c>
+      <c r="D6" s="12">
+        <v>9</v>
+      </c>
+      <c r="E6" s="32">
         <v>1</v>
       </c>
     </row>
@@ -980,12 +980,12 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="12">
+        <v>101</v>
+      </c>
+      <c r="D7" s="12">
+        <v>38</v>
+      </c>
+      <c r="E7" s="32">
         <v>1</v>
       </c>
     </row>
@@ -994,15 +994,15 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13">
+        <v>72</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1011,15 +1011,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13">
+        <v>73</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1028,15 +1028,15 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13">
+        <v>67</v>
+      </c>
+      <c r="D10" s="13">
+        <v>13</v>
+      </c>
+      <c r="E10" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1045,15 +1045,15 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="13">
+        <v>82</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1062,15 +1062,15 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="13">
+        <v>66</v>
+      </c>
+      <c r="D12" s="22">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
         <v>2</v>
       </c>
     </row>
@@ -1079,15 +1079,15 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="14">
+        <v>74</v>
+      </c>
+      <c r="D13" s="14">
+        <v>18</v>
+      </c>
+      <c r="E13" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1096,15 +1096,15 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="14">
+        <v>75</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1113,15 +1113,15 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="14">
+        <v>68</v>
+      </c>
+      <c r="D15" s="30">
+        <v>0</v>
+      </c>
+      <c r="E15" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1130,15 +1130,15 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="14">
+        <v>83</v>
+      </c>
+      <c r="D16" s="14">
+        <v>19</v>
+      </c>
+      <c r="E16" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1147,15 +1147,15 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="14">
+        <v>89</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1164,15 +1164,15 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="15">
+        <v>105</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1181,15 +1181,15 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="15">
+        <v>76</v>
+      </c>
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1198,15 +1198,15 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="15">
+        <v>69</v>
+      </c>
+      <c r="D20" s="15">
+        <v>23</v>
+      </c>
+      <c r="E20" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1215,15 +1215,15 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="15">
+        <v>84</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1232,15 +1232,15 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="15">
+        <v>66</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1249,15 +1249,15 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="15">
+        <v>102</v>
+      </c>
+      <c r="D23" s="15">
+        <v>27</v>
+      </c>
+      <c r="E23" s="35">
         <v>4</v>
       </c>
     </row>
@@ -1266,15 +1266,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="16">
+        <v>80</v>
+      </c>
+      <c r="D24" s="16">
+        <v>29</v>
+      </c>
+      <c r="E24" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1283,15 +1283,15 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="16">
+        <v>106</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1300,15 +1300,15 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="16">
+        <v>95</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1317,15 +1317,15 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="16">
+        <v>85</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1334,15 +1334,15 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="16">
+        <v>66</v>
+      </c>
+      <c r="D28" s="27">
+        <v>0</v>
+      </c>
+      <c r="E28" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1351,15 +1351,15 @@
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="16">
+        <v>103</v>
+      </c>
+      <c r="D29" s="27">
+        <v>0</v>
+      </c>
+      <c r="E29" s="36">
         <v>5</v>
       </c>
     </row>
@@ -1368,15 +1368,15 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="17">
+        <v>79</v>
+      </c>
+      <c r="D30" s="28">
+        <v>0</v>
+      </c>
+      <c r="E30" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1385,15 +1385,15 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="17">
+        <v>97</v>
+      </c>
+      <c r="D31" s="28">
+        <v>0</v>
+      </c>
+      <c r="E31" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1402,15 +1402,15 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="17">
+        <v>90</v>
+      </c>
+      <c r="D32" s="17">
+        <v>35</v>
+      </c>
+      <c r="E32" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1419,15 +1419,15 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="17">
+        <v>86</v>
+      </c>
+      <c r="D33" s="17">
+        <v>40</v>
+      </c>
+      <c r="E33" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1436,15 +1436,15 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="17">
+        <v>92</v>
+      </c>
+      <c r="D34" s="17">
+        <v>37</v>
+      </c>
+      <c r="E34" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1453,15 +1453,15 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="18">
+        <v>78</v>
+      </c>
+      <c r="D35" s="18">
+        <v>46</v>
+      </c>
+      <c r="E35" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1470,15 +1470,15 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" s="18">
+        <v>88</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1487,15 +1487,15 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E37" s="18">
+        <v>91</v>
+      </c>
+      <c r="D37" s="18">
+        <v>41</v>
+      </c>
+      <c r="E37" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1504,15 +1504,15 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="18">
+        <v>104</v>
+      </c>
+      <c r="D38" s="26">
+        <v>0</v>
+      </c>
+      <c r="E38" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1521,15 +1521,15 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" s="18">
+        <v>93</v>
+      </c>
+      <c r="D39" s="26">
+        <v>0</v>
+      </c>
+      <c r="E39" s="38">
         <v>7</v>
       </c>
     </row>
@@ -1538,15 +1538,15 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="19">
+        <v>98</v>
+      </c>
+      <c r="D40" s="21">
+        <v>0</v>
+      </c>
+      <c r="E40" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1555,15 +1555,15 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="19">
+        <v>87</v>
+      </c>
+      <c r="D41" s="21">
+        <v>0</v>
+      </c>
+      <c r="E41" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1572,15 +1572,15 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="19">
+        <v>94</v>
+      </c>
+      <c r="D42" s="21">
+        <v>0</v>
+      </c>
+      <c r="E42" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1589,15 +1589,15 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" s="19">
+        <v>96</v>
+      </c>
+      <c r="D43" s="19">
+        <v>46</v>
+      </c>
+      <c r="E43" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1606,15 +1606,15 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" s="19">
+        <v>66</v>
+      </c>
+      <c r="D44" s="21">
+        <v>0</v>
+      </c>
+      <c r="E44" s="39">
         <v>8</v>
       </c>
     </row>
@@ -1623,15 +1623,15 @@
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E45" s="20">
+        <v>38</v>
+      </c>
+      <c r="D45" s="25">
+        <v>0</v>
+      </c>
+      <c r="E45" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1640,15 +1640,15 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E46" s="20">
+        <v>38</v>
+      </c>
+      <c r="D46" s="25">
+        <v>0</v>
+      </c>
+      <c r="E46" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1657,15 +1657,15 @@
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E47" s="20">
+        <v>38</v>
+      </c>
+      <c r="D47" s="25">
+        <v>0</v>
+      </c>
+      <c r="E47" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1674,15 +1674,15 @@
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E48" s="20">
+        <v>99</v>
+      </c>
+      <c r="D48" s="20">
+        <v>51</v>
+      </c>
+      <c r="E48" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1691,15 +1691,15 @@
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E49" s="20">
+        <v>38</v>
+      </c>
+      <c r="D49" s="25">
+        <v>0</v>
+      </c>
+      <c r="E49" s="40">
         <v>9</v>
       </c>
     </row>
@@ -1708,15 +1708,15 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E50" s="21">
+        <v>38</v>
+      </c>
+      <c r="D50" s="24">
+        <v>0</v>
+      </c>
+      <c r="E50" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1725,15 +1725,15 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E51" s="21">
+        <v>38</v>
+      </c>
+      <c r="D51" s="24">
+        <v>0</v>
+      </c>
+      <c r="E51" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1742,15 +1742,15 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E52" s="21">
+        <v>38</v>
+      </c>
+      <c r="D52" s="24">
+        <v>0</v>
+      </c>
+      <c r="E52" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1759,15 +1759,15 @@
         <v>51</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E53" s="21">
+        <v>100</v>
+      </c>
+      <c r="D53" s="24">
+        <v>0</v>
+      </c>
+      <c r="E53" s="41">
         <v>10</v>
       </c>
     </row>
@@ -1776,20 +1776,23 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" s="21">
+        <v>38</v>
+      </c>
+      <c r="D54" s="24">
+        <v>0</v>
+      </c>
+      <c r="E54" s="41">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D4" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añade casos para semestre aprobado = 8, 9 o 10
</commit_message>
<xml_diff>
--- a/generador_ruta_critica/MallaCurricular.xlsx
+++ b/generador_ruta_critica/MallaCurricular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador_ruta_critica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285A9E4-41C0-45A2-8E1F-0B12872E6960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1B0002-FB96-43EC-A820-6E18513DBA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>CONTABILIDAD Y COSTOS</t>
   </si>
   <si>
-    <t>INTRODUCCIÓN A LA ECONOMÍA</t>
-  </si>
-  <si>
     <t>OPTIMIZACIÓN</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>ELECTRÓNICA Y ELECTROTECNIA</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN  A LA ECONOMÍA</t>
   </si>
 </sst>
 </file>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +963,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="12">
         <v>9</v>
@@ -980,7 +980,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="12">
         <v>38</v>
@@ -1048,7 +1048,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>57</v>
@@ -1133,7 +1133,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="14">
         <v>19</v>
@@ -1150,7 +1150,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>59</v>
@@ -1167,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>60</v>
@@ -1218,7 +1218,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>61</v>
@@ -1252,7 +1252,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1269,7 +1269,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="16">
         <v>29</v>
@@ -1286,7 +1286,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>62</v>
@@ -1303,7 +1303,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>63</v>
@@ -1320,7 +1320,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D27" s="16" t="s">
         <v>64</v>
@@ -1354,7 +1354,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" s="27">
         <v>0</v>
@@ -1371,7 +1371,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="D30" s="28">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" s="28">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="17">
         <v>35</v>
@@ -1422,7 +1422,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="17">
         <v>40</v>
@@ -1439,7 +1439,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="17">
         <v>37</v>
@@ -1473,7 +1473,7 @@
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>65</v>
@@ -1490,7 +1490,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="18">
         <v>41</v>
@@ -1507,7 +1507,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="26">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="26">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="21">
         <v>0</v>
@@ -1558,7 +1558,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="21">
         <v>0</v>
@@ -1575,7 +1575,7 @@
         <v>36</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" s="21">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D43" s="19">
         <v>46</v>
@@ -1677,7 +1677,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D48" s="20">
         <v>51</v>
@@ -1762,7 +1762,7 @@
         <v>47</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" s="24">
         <v>0</v>

</xml_diff>